<commit_message>
[expression] - [CSV]: [`merge(var,keyColumns)`] now supports multiple "key" columns so that one can merge 2 CSV content based on multiple keys. Note that both CSV content must contain header (i.e. parsed with `header=true`).
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/showcase/artifact/data/xml-showcase.data.xlsx
+++ b/src/test/resources/showcase/artifact/data/xml-showcase.data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10909"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/nexial-core/src/test/resources/showcase/artifact/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lium183/projects/nexial/nexial-core/src/test/resources/showcase/artifact/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E5CBB5D-116C-7C49-8BAB-D4AFBA53169D}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79537D91-F106-EE44-A3B1-B1426E1B24AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="51200" windowHeight="10520" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="10520" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
@@ -49,20 +49,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
   <si>
     <t>true</t>
   </si>
   <si>
-    <t>800</t>
-  </si>
-  <si>
     <t>,</t>
   </si>
   <si>
-    <t>600</t>
-  </si>
-  <si>
     <t>false</t>
   </si>
   <si>
@@ -142,6 +136,9 @@
   </si>
   <si>
     <t>$(syspath|data|fullpath)/xml-showcase-test1.xml</t>
+  </si>
+  <si>
+    <t>0</t>
   </si>
 </sst>
 </file>
@@ -680,7 +677,7 @@
   <dimension ref="A1:AAA16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
@@ -694,7 +691,7 @@
   <sheetData>
     <row r="1" spans="1:703">
       <c r="A1" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -704,139 +701,139 @@
     </row>
     <row r="2" spans="1:703">
       <c r="A2" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="HA2" s="6"/>
       <c r="AAA2" s="6"/>
     </row>
     <row r="3" spans="1:703">
       <c r="A3" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="HA3" s="4"/>
       <c r="AAA3" s="5"/>
     </row>
     <row r="4" spans="1:703">
       <c r="A4" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="HA4" s="4"/>
       <c r="AAA4" s="5"/>
     </row>
     <row r="5" spans="1:703">
       <c r="A5" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="HA5" s="4"/>
       <c r="AAA5" s="5"/>
     </row>
     <row r="6" spans="1:703">
       <c r="A6" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="HA6" s="4"/>
       <c r="AAA6" s="5"/>
     </row>
     <row r="7" spans="1:703">
       <c r="A7" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="HA7" s="4"/>
       <c r="AAA7" s="5"/>
     </row>
     <row r="8" spans="1:703">
       <c r="A8" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="HA8" s="4"/>
       <c r="AAA8" s="5"/>
     </row>
     <row r="9" spans="1:703">
       <c r="A9" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="HA9" s="4"/>
       <c r="AAA9" s="5"/>
     </row>
     <row r="10" spans="1:703">
       <c r="A10" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C10" s="2"/>
     </row>
     <row r="11" spans="1:703">
       <c r="A11" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:703">
       <c r="A12" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:703">
       <c r="A13" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:703">
       <c r="A14" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:703">
       <c r="A15" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:703">
       <c r="A16" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>